<commit_message>
all working as intended
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Bubblesort</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>sorted</t>
+  </si>
+  <si>
+    <t>#error</t>
+  </si>
+  <si>
+    <t>inverted</t>
+  </si>
+  <si>
+    <t>partly sorted</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +454,9 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
       <c r="E2" s="1">
         <v>9</v>
       </c>
@@ -463,7 +474,9 @@
       <c r="C3" s="1">
         <v>483</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>37</v>
+      </c>
       <c r="E3" s="1">
         <v>860</v>
       </c>
@@ -478,7 +491,9 @@
       <c r="C4" s="1">
         <v>49780</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>482</v>
+      </c>
       <c r="E4" s="1">
         <v>84328</v>
       </c>
@@ -509,7 +524,9 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
       <c r="E7" s="1">
         <v>9</v>
       </c>
@@ -527,7 +544,9 @@
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>461</v>
+      </c>
       <c r="E8" s="1">
         <v>860</v>
       </c>
@@ -542,7 +561,9 @@
       <c r="C9" s="1">
         <v>56</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="1">
         <v>84892</v>
       </c>
@@ -555,6 +576,122 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1569</v>
+      </c>
+      <c r="C13" s="1">
+        <v>992</v>
+      </c>
+      <c r="D13" s="1">
+        <v>744</v>
+      </c>
+      <c r="E13" s="1">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>155383</v>
+      </c>
+      <c r="C14" s="1">
+        <v>99046</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>92703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>